<commit_message>
resend verif code, subcat travel, eye toggle in password fields
</commit_message>
<xml_diff>
--- a/frontend/public/template.xlsx
+++ b/frontend/public/template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Nana world\thesis\frontend\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B166D32-EECD-4F6D-94F2-091B1D0F0B3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{411CC9FD-2D10-4C68-845D-FFF3B0D5B7D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2448" windowWidth="21600" windowHeight="11232" xr2:uid="{AFC31B34-29BE-48B1-94A9-DC4AF8DEDAE9}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{AFC31B34-29BE-48B1-94A9-DC4AF8DEDAE9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>Amount</t>
   </si>
@@ -123,6 +123,9 @@
   </si>
   <si>
     <t>savings</t>
+  </si>
+  <si>
+    <t>travel</t>
   </si>
 </sst>
 </file>
@@ -511,10 +514,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6760371-DD65-40D4-A1BA-49A06C17F87E}">
-  <dimension ref="A1:I25"/>
+  <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -579,7 +582,7 @@
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="I8" s="2" t="s">
+      <c r="I8" s="1" t="s">
         <v>11</v>
       </c>
     </row>
@@ -639,32 +642,37 @@
       </c>
     </row>
     <row r="20" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I20" t="s">
-        <v>23</v>
+      <c r="I20" s="2" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="21" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I21" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="22" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I22" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="23" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I23" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="24" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I24" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="25" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I25" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="26" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I26" t="s">
         <v>28</v>
       </c>
     </row>

</xml_diff>